<commit_message>
Feat: QR code added
</commit_message>
<xml_diff>
--- a/public/list.xlsx
+++ b/public/list.xlsx
@@ -150,7 +150,7 @@
     <t>OYINDAMOLA, OKIKIOLUWA &amp; TIWALOLA</t>
   </si>
   <si>
-    <t>0808027704160</t>
+    <t>08027704160</t>
   </si>
   <si>
     <t>OMOJIADE</t>
@@ -222,7 +222,7 @@
     <t>TIRENI &amp; TISHE</t>
   </si>
   <si>
-    <t>0803762863</t>
+    <t>08037262863</t>
   </si>
   <si>
     <t>ADETIRAN</t>
@@ -279,7 +279,7 @@
     <t>08069789336</t>
   </si>
   <si>
-    <t>ADEWOLE</t>
+    <t xml:space="preserve">ADEWOLE  </t>
   </si>
   <si>
     <t>TEMILOLUWA  &amp; ADESOLA</t>
@@ -1280,7 +1280,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1321,6 +1321,9 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2389,7 +2392,7 @@
       <c r="D22" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="13" t="s">
         <v>68</v>
       </c>
       <c r="F22" s="9">
@@ -2648,7 +2651,7 @@
       <c r="A29" s="5">
         <v>28.0</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="14" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="5"/>
@@ -3149,7 +3152,7 @@
       <c r="D42" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="15" t="s">
         <v>128</v>
       </c>
       <c r="F42" s="9">
@@ -3605,7 +3608,7 @@
       <c r="D54" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="16" t="s">
         <v>164</v>
       </c>
       <c r="F54" s="9">
@@ -3643,7 +3646,7 @@
       <c r="D55" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E55" s="16" t="s">
         <v>167</v>
       </c>
       <c r="F55" s="9">
@@ -3678,10 +3681,10 @@
         <v>168</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="18">
         <v>8.023886616E9</v>
       </c>
       <c r="F56" s="9">
@@ -3719,7 +3722,7 @@
       <c r="D57" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="18">
         <v>8.033556554E9</v>
       </c>
       <c r="F57" s="9">
@@ -3757,7 +3760,7 @@
       <c r="D58" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="E58" s="18">
+      <c r="E58" s="19">
         <v>8.062690098E9</v>
       </c>
       <c r="F58" s="9">
@@ -3795,7 +3798,7 @@
       <c r="D59" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="20" t="s">
         <v>175</v>
       </c>
       <c r="F59" s="9">
@@ -3833,7 +3836,7 @@
       <c r="D60" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="20" t="s">
         <v>178</v>
       </c>
       <c r="F60" s="9">
@@ -3871,7 +3874,7 @@
       <c r="D61" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="20" t="s">
         <v>181</v>
       </c>
       <c r="F61" s="9">
@@ -3906,10 +3909,10 @@
         <v>182</v>
       </c>
       <c r="C62" s="5"/>
-      <c r="D62" s="20" t="s">
+      <c r="D62" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="20" t="s">
         <v>184</v>
       </c>
       <c r="F62" s="9">
@@ -3947,7 +3950,7 @@
       <c r="D63" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="20" t="s">
         <v>187</v>
       </c>
       <c r="F63" s="9">
@@ -3985,7 +3988,7 @@
       <c r="D64" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="20" t="s">
         <v>190</v>
       </c>
       <c r="F64" s="9">
@@ -4023,7 +4026,7 @@
       <c r="D65" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="E65" s="19" t="s">
+      <c r="E65" s="20" t="s">
         <v>193</v>
       </c>
       <c r="F65" s="9">
@@ -4061,7 +4064,7 @@
       <c r="D66" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="E66" s="19" t="s">
+      <c r="E66" s="20" t="s">
         <v>196</v>
       </c>
       <c r="F66" s="9">
@@ -4099,7 +4102,7 @@
       <c r="D67" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E67" s="19" t="s">
+      <c r="E67" s="20" t="s">
         <v>199</v>
       </c>
       <c r="F67" s="9">
@@ -4137,7 +4140,7 @@
       <c r="D68" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="E68" s="19" t="s">
+      <c r="E68" s="20" t="s">
         <v>202</v>
       </c>
       <c r="F68" s="9">
@@ -4172,10 +4175,10 @@
         <v>203</v>
       </c>
       <c r="C69" s="5"/>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="20" t="s">
         <v>205</v>
       </c>
       <c r="F69" s="9">
@@ -4213,7 +4216,7 @@
       <c r="D70" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="E70" s="19" t="s">
+      <c r="E70" s="20" t="s">
         <v>208</v>
       </c>
       <c r="F70" s="9">
@@ -4251,7 +4254,7 @@
       <c r="D71" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="20" t="s">
         <v>211</v>
       </c>
       <c r="F71" s="2">
@@ -4289,7 +4292,7 @@
       <c r="D72" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="E72" s="19" t="s">
+      <c r="E72" s="20" t="s">
         <v>214</v>
       </c>
       <c r="F72" s="2">
@@ -4327,7 +4330,7 @@
       <c r="D73" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="E73" s="19" t="s">
+      <c r="E73" s="20" t="s">
         <v>217</v>
       </c>
       <c r="F73" s="2">
@@ -4365,7 +4368,7 @@
       <c r="D74" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="E74" s="19" t="s">
+      <c r="E74" s="20" t="s">
         <v>220</v>
       </c>
       <c r="F74" s="2">
@@ -4403,7 +4406,7 @@
       <c r="D75" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="E75" s="19" t="s">
+      <c r="E75" s="20" t="s">
         <v>223</v>
       </c>
       <c r="F75" s="2">
@@ -4441,7 +4444,7 @@
       <c r="D76" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E76" s="20" t="s">
         <v>226</v>
       </c>
       <c r="F76" s="2">
@@ -4479,7 +4482,7 @@
       <c r="D77" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E77" s="20" t="s">
         <v>229</v>
       </c>
       <c r="F77" s="2">
@@ -4517,7 +4520,7 @@
       <c r="D78" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E78" s="20" t="s">
         <v>231</v>
       </c>
       <c r="F78" s="2">
@@ -4555,7 +4558,7 @@
       <c r="D79" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="20" t="s">
         <v>234</v>
       </c>
       <c r="F79" s="2">
@@ -4593,7 +4596,7 @@
       <c r="D80" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E80" s="20" t="s">
         <v>237</v>
       </c>
       <c r="F80" s="2">
@@ -4631,7 +4634,7 @@
       <c r="D81" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="E81" s="19" t="s">
+      <c r="E81" s="20" t="s">
         <v>240</v>
       </c>
       <c r="F81" s="2">
@@ -4669,7 +4672,7 @@
       <c r="D82" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="E82" s="19" t="s">
+      <c r="E82" s="20" t="s">
         <v>243</v>
       </c>
       <c r="F82" s="2">
@@ -4743,7 +4746,7 @@
       <c r="D84" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="E84" s="19" t="s">
+      <c r="E84" s="20" t="s">
         <v>248</v>
       </c>
       <c r="F84" s="2">
@@ -4781,7 +4784,7 @@
       <c r="D85" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="E85" s="19" t="s">
+      <c r="E85" s="20" t="s">
         <v>251</v>
       </c>
       <c r="F85" s="2">
@@ -4819,7 +4822,7 @@
       <c r="D86" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="E86" s="19" t="s">
+      <c r="E86" s="20" t="s">
         <v>254</v>
       </c>
       <c r="F86" s="2">
@@ -4857,7 +4860,7 @@
       <c r="D87" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="20" t="s">
         <v>257</v>
       </c>
       <c r="F87" s="2">
@@ -4895,7 +4898,7 @@
       <c r="D88" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="20" t="s">
         <v>260</v>
       </c>
       <c r="F88" s="2">
@@ -4933,7 +4936,7 @@
       <c r="D89" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E89" s="19">
+      <c r="E89" s="20">
         <v>15073193312</v>
       </c>
       <c r="F89" s="2">
@@ -4971,7 +4974,7 @@
       <c r="D90" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="E90" s="19" t="s">
+      <c r="E90" s="20" t="s">
         <v>265</v>
       </c>
       <c r="F90" s="2">
@@ -5119,7 +5122,7 @@
       <c r="D94" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="E94" s="19" t="s">
+      <c r="E94" s="20" t="s">
         <v>274</v>
       </c>
       <c r="F94" s="2">
@@ -5157,7 +5160,7 @@
       <c r="D95" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E95" s="19" t="s">
+      <c r="E95" s="20" t="s">
         <v>277</v>
       </c>
       <c r="F95" s="2">
@@ -5195,7 +5198,7 @@
       <c r="D96" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="E96" s="19" t="s">
+      <c r="E96" s="20" t="s">
         <v>280</v>
       </c>
       <c r="F96" s="2">
@@ -5233,7 +5236,7 @@
       <c r="D97" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="E97" s="19" t="s">
+      <c r="E97" s="20" t="s">
         <v>282</v>
       </c>
       <c r="F97" s="2">
@@ -5271,7 +5274,7 @@
       <c r="D98" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="E98" s="19" t="s">
+      <c r="E98" s="20" t="s">
         <v>285</v>
       </c>
       <c r="F98" s="2">
@@ -5309,7 +5312,7 @@
       <c r="D99" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="E99" s="19" t="s">
+      <c r="E99" s="20" t="s">
         <v>288</v>
       </c>
       <c r="F99" s="2">
@@ -5347,7 +5350,7 @@
       <c r="D100" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="E100" s="19" t="s">
+      <c r="E100" s="20" t="s">
         <v>291</v>
       </c>
       <c r="F100" s="2">
@@ -5385,7 +5388,7 @@
       <c r="D101" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="E101" s="19" t="s">
+      <c r="E101" s="20" t="s">
         <v>294</v>
       </c>
       <c r="F101" s="2">
@@ -5423,7 +5426,7 @@
       <c r="D102" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="E102" s="19" t="s">
+      <c r="E102" s="20" t="s">
         <v>297</v>
       </c>
       <c r="F102" s="2">
@@ -5461,7 +5464,7 @@
       <c r="D103" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="E103" s="19" t="s">
+      <c r="E103" s="20" t="s">
         <v>300</v>
       </c>
       <c r="F103" s="2">
@@ -5499,7 +5502,7 @@
       <c r="D104" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="E104" s="19" t="s">
+      <c r="E104" s="20" t="s">
         <v>303</v>
       </c>
       <c r="F104" s="2">
@@ -5537,10 +5540,7 @@
       <c r="D105" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="E105" s="19">
-        <f>15073193312</f>
-        <v>15073193312</v>
-      </c>
+      <c r="E105" s="20"/>
       <c r="F105" s="2">
         <v>1.0</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="D106" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="E106" s="19" t="s">
+      <c r="E106" s="20" t="s">
         <v>308</v>
       </c>
       <c r="F106" s="2">
@@ -5650,7 +5650,7 @@
       <c r="D108" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="E108" s="21" t="s">
+      <c r="E108" s="22" t="s">
         <v>313</v>
       </c>
       <c r="F108" s="2">
@@ -5688,7 +5688,7 @@
       <c r="D109" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="E109" s="19" t="s">
+      <c r="E109" s="20" t="s">
         <v>316</v>
       </c>
       <c r="F109" s="2">
@@ -5726,7 +5726,7 @@
       <c r="D110" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="E110" s="19" t="s">
+      <c r="E110" s="20" t="s">
         <v>319</v>
       </c>
       <c r="F110" s="2">
@@ -5764,7 +5764,7 @@
       <c r="D111" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="E111" s="19" t="s">
+      <c r="E111" s="20" t="s">
         <v>322</v>
       </c>
       <c r="F111" s="2">
@@ -5802,7 +5802,7 @@
       <c r="D112" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E112" s="20" t="s">
         <v>325</v>
       </c>
       <c r="F112" s="2">
@@ -5840,7 +5840,7 @@
       <c r="D113" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="E113" s="19" t="s">
+      <c r="E113" s="20" t="s">
         <v>328</v>
       </c>
       <c r="F113" s="2">
@@ -5878,7 +5878,7 @@
       <c r="D114" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="E114" s="19" t="s">
+      <c r="E114" s="20" t="s">
         <v>331</v>
       </c>
       <c r="F114" s="2">
@@ -5916,7 +5916,7 @@
       <c r="D115" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="E115" s="19" t="s">
+      <c r="E115" s="20" t="s">
         <v>334</v>
       </c>
       <c r="F115" s="2">
@@ -5954,7 +5954,7 @@
       <c r="D116" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="E116" s="19" t="s">
+      <c r="E116" s="20" t="s">
         <v>337</v>
       </c>
       <c r="F116" s="2">
@@ -5992,7 +5992,7 @@
       <c r="D117" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="E117" s="19" t="s">
+      <c r="E117" s="20" t="s">
         <v>340</v>
       </c>
       <c r="F117" s="2">
@@ -6030,7 +6030,7 @@
       <c r="D118" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="E118" s="19" t="s">
+      <c r="E118" s="20" t="s">
         <v>343</v>
       </c>
       <c r="F118" s="2">
@@ -6068,7 +6068,7 @@
       <c r="D119" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="E119" s="19" t="s">
+      <c r="E119" s="20" t="s">
         <v>346</v>
       </c>
       <c r="F119" s="2">
@@ -6106,7 +6106,7 @@
       <c r="D120" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="E120" s="19" t="s">
+      <c r="E120" s="20" t="s">
         <v>349</v>
       </c>
       <c r="F120" s="2">
@@ -6144,7 +6144,7 @@
       <c r="D121" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="E121" s="19" t="s">
+      <c r="E121" s="20" t="s">
         <v>352</v>
       </c>
       <c r="F121" s="2">
@@ -6182,7 +6182,7 @@
       <c r="D122" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="E122" s="19" t="s">
+      <c r="E122" s="20" t="s">
         <v>355</v>
       </c>
       <c r="F122" s="2">
@@ -6220,7 +6220,7 @@
       <c r="D123" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="E123" s="19" t="s">
+      <c r="E123" s="20" t="s">
         <v>358</v>
       </c>
       <c r="F123" s="2">
@@ -6251,14 +6251,14 @@
       <c r="A124" s="5">
         <v>124.0</v>
       </c>
-      <c r="B124" s="22" t="s">
+      <c r="B124" s="23" t="s">
         <v>359</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="E124" s="22">
+      <c r="E124" s="23">
         <v>8.051931418E9</v>
       </c>
       <c r="F124" s="2">
@@ -6289,14 +6289,14 @@
       <c r="A125" s="5">
         <v>125.0</v>
       </c>
-      <c r="B125" s="22" t="s">
+      <c r="B125" s="23" t="s">
         <v>361</v>
       </c>
       <c r="C125" s="5"/>
       <c r="D125" s="5" t="s">
         <v>362</v>
       </c>
-      <c r="E125" s="22">
+      <c r="E125" s="23">
         <v>8.067651953E9</v>
       </c>
       <c r="F125" s="2">
@@ -6327,14 +6327,14 @@
       <c r="A126" s="5">
         <v>126.0</v>
       </c>
-      <c r="B126" s="22" t="s">
+      <c r="B126" s="23" t="s">
         <v>363</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="E126" s="22">
+      <c r="E126" s="23">
         <v>8.069744949E9</v>
       </c>
       <c r="F126" s="2">
@@ -6365,7 +6365,7 @@
       <c r="A127" s="5">
         <v>127.0</v>
       </c>
-      <c r="B127" s="22" t="s">
+      <c r="B127" s="23" t="s">
         <v>365</v>
       </c>
       <c r="C127" s="5"/>
@@ -6403,11 +6403,11 @@
       <c r="A128" s="5">
         <v>128.0</v>
       </c>
-      <c r="B128" s="22" t="s">
+      <c r="B128" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="C128" s="22"/>
-      <c r="D128" s="22" t="s">
+      <c r="C128" s="23"/>
+      <c r="D128" s="23" t="s">
         <v>368</v>
       </c>
       <c r="E128" s="5">
@@ -6441,11 +6441,11 @@
       <c r="A129" s="5">
         <v>129.0</v>
       </c>
-      <c r="B129" s="22" t="s">
+      <c r="B129" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="C129" s="22"/>
-      <c r="D129" s="22" t="s">
+      <c r="C129" s="23"/>
+      <c r="D129" s="23" t="s">
         <v>370</v>
       </c>
       <c r="E129" s="5">
@@ -6479,11 +6479,11 @@
       <c r="A130" s="5">
         <v>130.0</v>
       </c>
-      <c r="B130" s="22" t="s">
+      <c r="B130" s="23" t="s">
         <v>371</v>
       </c>
       <c r="C130" s="5"/>
-      <c r="D130" s="22" t="s">
+      <c r="D130" s="23" t="s">
         <v>372</v>
       </c>
       <c r="E130" s="5">
@@ -6514,17 +6514,17 @@
       <c r="Z130" s="4"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="23">
+      <c r="A131" s="24">
         <v>131.0</v>
       </c>
-      <c r="B131" s="17" t="s">
+      <c r="B131" s="18" t="s">
         <v>373</v>
       </c>
       <c r="C131" s="5"/>
-      <c r="D131" s="17" t="s">
+      <c r="D131" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="E131" s="23">
+      <c r="E131" s="24">
         <v>8.034846488E9</v>
       </c>
       <c r="F131" s="2">
@@ -6553,9 +6553,9 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="5"/>
-      <c r="B132" s="22"/>
+      <c r="B132" s="23"/>
       <c r="C132" s="5"/>
-      <c r="D132" s="22"/>
+      <c r="D132" s="23"/>
       <c r="E132" s="5"/>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
@@ -6583,9 +6583,9 @@
       <c r="A133" s="5">
         <v>131.0</v>
       </c>
-      <c r="B133" s="22"/>
+      <c r="B133" s="23"/>
       <c r="C133" s="5"/>
-      <c r="D133" s="22" t="s">
+      <c r="D133" s="23" t="s">
         <v>375</v>
       </c>
       <c r="E133" s="5"/>
@@ -6615,9 +6615,9 @@
       <c r="A134" s="5">
         <v>132.0</v>
       </c>
-      <c r="B134" s="22"/>
-      <c r="C134" s="22"/>
-      <c r="D134" s="22" t="s">
+      <c r="B134" s="23"/>
+      <c r="C134" s="23"/>
+      <c r="D134" s="23" t="s">
         <v>376</v>
       </c>
       <c r="E134" s="5"/>
@@ -6647,9 +6647,9 @@
       <c r="A135" s="5">
         <v>133.0</v>
       </c>
-      <c r="B135" s="22"/>
-      <c r="C135" s="22"/>
-      <c r="D135" s="22" t="s">
+      <c r="B135" s="23"/>
+      <c r="C135" s="23"/>
+      <c r="D135" s="23" t="s">
         <v>377</v>
       </c>
       <c r="E135" s="5"/>
@@ -6679,12 +6679,12 @@
       <c r="A136" s="5">
         <v>134.0</v>
       </c>
-      <c r="B136" s="22"/>
-      <c r="C136" s="22"/>
-      <c r="D136" s="22" t="s">
+      <c r="B136" s="23"/>
+      <c r="C136" s="23"/>
+      <c r="D136" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="E136" s="19" t="s">
+      <c r="E136" s="20" t="s">
         <v>379</v>
       </c>
       <c r="F136" s="2">
@@ -6715,9 +6715,9 @@
       <c r="A137" s="5">
         <v>135.0</v>
       </c>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22"/>
-      <c r="D137" s="22" t="s">
+      <c r="B137" s="23"/>
+      <c r="C137" s="23"/>
+      <c r="D137" s="23" t="s">
         <v>380</v>
       </c>
       <c r="E137" s="5"/>
@@ -6747,9 +6747,9 @@
       <c r="A138" s="5">
         <v>136.0</v>
       </c>
-      <c r="B138" s="22"/>
-      <c r="C138" s="22"/>
-      <c r="D138" s="22" t="s">
+      <c r="B138" s="23"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23" t="s">
         <v>381</v>
       </c>
       <c r="E138" s="5"/>
@@ -6779,9 +6779,9 @@
       <c r="A139" s="5">
         <v>137.0</v>
       </c>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
-      <c r="D139" s="22" t="s">
+      <c r="B139" s="23"/>
+      <c r="C139" s="23"/>
+      <c r="D139" s="23" t="s">
         <v>382</v>
       </c>
       <c r="E139" s="5"/>
@@ -6811,9 +6811,9 @@
       <c r="A140" s="5">
         <v>138.0</v>
       </c>
-      <c r="B140" s="22"/>
-      <c r="C140" s="22"/>
-      <c r="D140" s="22" t="s">
+      <c r="B140" s="23"/>
+      <c r="C140" s="23"/>
+      <c r="D140" s="23" t="s">
         <v>383</v>
       </c>
       <c r="E140" s="5"/>

</xml_diff>